<commit_message>
Versión 3.1, Oscar David funcional, GUI actualizada
</commit_message>
<xml_diff>
--- a/andina-maxiconsumo.xlsx
+++ b/andina-maxiconsumo.xlsx
@@ -508,7 +508,7 @@
     <col min="15" max="15" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1">
         <v>7509552790139</v>
       </c>
@@ -551,7 +551,7 @@
       </c>
       <c r="O1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1">
         <v>7790010002516</v>
       </c>
@@ -596,7 +596,7 @@
       </c>
       <c r="O2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1">
         <v>7790740000509</v>
       </c>
@@ -641,7 +641,7 @@
       </c>
       <c r="O3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1">
         <v>7790740000684</v>
       </c>
@@ -686,7 +686,7 @@
       </c>
       <c r="O4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1">
         <v>7791293042848</v>
       </c>
@@ -731,7 +731,7 @@
       </c>
       <c r="O5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1">
         <v>7791293043548</v>
       </c>
@@ -776,7 +776,7 @@
       </c>
       <c r="O6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1">
         <v>7791293045931</v>
       </c>
@@ -821,7 +821,7 @@
       </c>
       <c r="O7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1">
         <v>7791293042077</v>
       </c>
@@ -866,7 +866,7 @@
       </c>
       <c r="O8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1">
         <v>7791293044590</v>
       </c>
@@ -911,7 +911,7 @@
       </c>
       <c r="O9" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1">
         <v>7791293039862</v>
       </c>
@@ -956,7 +956,7 @@
       </c>
       <c r="O10" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1">
         <v>7794000006164</v>
       </c>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="O11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1">
         <v>7794000006324</v>
       </c>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="O12" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1">
         <v>7791866000381</v>
       </c>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="O13" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1">
         <v>7794000006096</v>
       </c>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="O14" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1">
         <v>7794000006058</v>
       </c>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="O15" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
@@ -1198,7 +1198,7 @@
       <c r="N16" s="6"/>
       <c r="O16" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
@@ -1215,7 +1215,7 @@
       <c r="N17" s="6"/>
       <c r="O17" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>

</xml_diff>